<commit_message>
C3 on C3 incorporated
</commit_message>
<xml_diff>
--- a/Codes/Multiple ANN models/Best_Models_from_C1_and_C2/All_Model_details_C1onC2.xlsx
+++ b/Codes/Multiple ANN models/Best_Models_from_C1_and_C2/All_Model_details_C1onC2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Model</t>
   </si>
@@ -52,6 +52,9 @@
     <t>%error(Ksym_Lam)</t>
   </si>
   <si>
+    <t>ANN(2HL-14,15 Nodes)</t>
+  </si>
+  <si>
     <t>ANN(2HL-14,18 Nodes)</t>
   </si>
   <si>
@@ -61,9 +64,27 @@
     <t>ANN(2HL-14,20 Nodes)</t>
   </si>
   <si>
+    <t>ANN(2HL-15,14 Nodes)</t>
+  </si>
+  <si>
+    <t>ANN(2HL-15,15 Nodes)</t>
+  </si>
+  <si>
+    <t>ANN(2HL-15,18 Nodes)</t>
+  </si>
+  <si>
+    <t>ANN(2HL-15,19 Nodes)</t>
+  </si>
+  <si>
+    <t>ANN(2HL-16,12 Nodes)</t>
+  </si>
+  <si>
     <t>ANN(2HL-16,14 Nodes)</t>
   </si>
   <si>
+    <t>ANN(2HL-16,15 Nodes)</t>
+  </si>
+  <si>
     <t>ANN(2HL-16,17 Nodes)</t>
   </si>
   <si>
@@ -73,6 +94,15 @@
     <t>ANN(2HL-16,19 Nodes)</t>
   </si>
   <si>
+    <t>ANN(2HL-16,20 Nodes)</t>
+  </si>
+  <si>
+    <t>ANN(2HL-17,13 Nodes)</t>
+  </si>
+  <si>
+    <t>ANN(2HL-17,14 Nodes)</t>
+  </si>
+  <si>
     <t>ANN(2HL-17,15 Nodes)</t>
   </si>
   <si>
@@ -88,6 +118,15 @@
     <t>ANN(2HL-17,19 Nodes)</t>
   </si>
   <si>
+    <t>ANN(2HL-18,10 Nodes)</t>
+  </si>
+  <si>
+    <t>ANN(2HL-18,11 Nodes)</t>
+  </si>
+  <si>
+    <t>ANN(2HL-18,12 Nodes)</t>
+  </si>
+  <si>
     <t>ANN(2HL-18,13 Nodes)</t>
   </si>
   <si>
@@ -103,6 +142,9 @@
     <t>ANN(2HL-18,17 Nodes)</t>
   </si>
   <si>
+    <t>ANN(2HL-18,18 Nodes)</t>
+  </si>
+  <si>
     <t>ANN(2HL-18,19 Nodes)</t>
   </si>
   <si>
@@ -118,9 +160,15 @@
     <t>ANN(2HL-19,14 Nodes)</t>
   </si>
   <si>
+    <t>ANN(2HL-19,15 Nodes)</t>
+  </si>
+  <si>
     <t>ANN(2HL-19,16 Nodes)</t>
   </si>
   <si>
+    <t>ANN(2HL-19,17 Nodes)</t>
+  </si>
+  <si>
     <t>ANN(2HL-19,18 Nodes)</t>
   </si>
   <si>
@@ -136,10 +184,16 @@
     <t>ANN(2HL-20,13 Nodes)</t>
   </si>
   <si>
+    <t>ANN(2HL-20,14 Nodes)</t>
+  </si>
+  <si>
     <t>ANN(2HL-20,15 Nodes)</t>
   </si>
   <si>
     <t>ANN(2HL-20,16 Nodes)</t>
+  </si>
+  <si>
+    <t>ANN(2HL-20,17 Nodes)</t>
   </si>
   <si>
     <t>ANN(2HL-20,18 Nodes)</t>
@@ -506,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -558,37 +612,37 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>14.22632968678037</v>
+        <v>14.9141540175411</v>
       </c>
       <c r="D2">
-        <v>0.02322829175163837</v>
+        <v>0.02206194985507051</v>
       </c>
       <c r="E2">
-        <v>0.2035273981204176</v>
+        <v>0.2091560036803448</v>
       </c>
       <c r="F2">
-        <v>24.63987431208981</v>
+        <v>25.83121633243979</v>
       </c>
       <c r="G2">
-        <v>0.9525311120684097</v>
+        <v>0.9518463777851086</v>
       </c>
       <c r="H2">
         <v>0.8305331942045113</v>
       </c>
       <c r="I2">
-        <v>0.8503489732284062</v>
+        <v>0.83808643732747</v>
       </c>
       <c r="J2">
-        <v>0.02385910540622583</v>
+        <v>0.009094450619993845</v>
       </c>
       <c r="K2">
         <v>0.8566798373674943</v>
       </c>
       <c r="L2">
-        <v>0.8749175388118806</v>
+        <v>0.8685775638322429</v>
       </c>
       <c r="M2">
-        <v>0.02128881835299081</v>
+        <v>0.01388818312954504</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -599,37 +653,37 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>14.67191314740286</v>
+        <v>14.37232379091544</v>
       </c>
       <c r="D3">
-        <v>0.02306006696393327</v>
+        <v>0.02218022829756752</v>
       </c>
       <c r="E3">
-        <v>0.2230586379921557</v>
+        <v>0.2110018152374424</v>
       </c>
       <c r="F3">
-        <v>25.41150958310287</v>
+        <v>24.89269088958005</v>
       </c>
       <c r="G3">
-        <v>0.9475554503304965</v>
+        <v>0.9519830454534075</v>
       </c>
       <c r="H3">
         <v>0.8305331942045113</v>
       </c>
       <c r="I3">
-        <v>0.8455171747978925</v>
+        <v>0.8388637108743182</v>
       </c>
       <c r="J3">
-        <v>0.01804139882420095</v>
+        <v>0.01003032356555706</v>
       </c>
       <c r="K3">
         <v>0.8566798373674943</v>
       </c>
       <c r="L3">
-        <v>0.8724671015912445</v>
+        <v>0.8630949814204836</v>
       </c>
       <c r="M3">
-        <v>0.01842842977635981</v>
+        <v>0.007488379874449323</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -640,37 +694,37 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>15.08264604732376</v>
+        <v>14.96143418091951</v>
       </c>
       <c r="D4">
-        <v>0.02097406970371253</v>
+        <v>0.02208613998406549</v>
       </c>
       <c r="E4">
-        <v>0.2064350833641541</v>
+        <v>0.2057813203867268</v>
       </c>
       <c r="F4">
-        <v>26.12308519320237</v>
+        <v>25.91313768150358</v>
       </c>
       <c r="G4">
-        <v>0.9535801880692593</v>
+        <v>0.9525281768779587</v>
       </c>
       <c r="H4">
         <v>0.8305331942045113</v>
       </c>
       <c r="I4">
-        <v>0.8405262444399488</v>
+        <v>0.8368933868646355</v>
       </c>
       <c r="J4">
-        <v>0.01203209011412108</v>
+        <v>0.007657963227124285</v>
       </c>
       <c r="K4">
         <v>0.8566798373674943</v>
       </c>
       <c r="L4">
-        <v>0.8656518300329739</v>
+        <v>0.8653758106108898</v>
       </c>
       <c r="M4">
-        <v>0.01047298217388859</v>
+        <v>0.01015078546743605</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -681,37 +735,37 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>14.3190650400951</v>
+        <v>14.97766183632132</v>
       </c>
       <c r="D5">
-        <v>0.02091381960656586</v>
+        <v>0.0196565875068293</v>
       </c>
       <c r="E5">
-        <v>0.1970481706151171</v>
+        <v>0.1994921902261521</v>
       </c>
       <c r="F5">
-        <v>24.80055655621515</v>
+        <v>25.94129678204609</v>
       </c>
       <c r="G5">
-        <v>0.9567634718629306</v>
+        <v>0.9568108120973831</v>
       </c>
       <c r="H5">
         <v>0.8305331942045113</v>
       </c>
       <c r="I5">
-        <v>0.8378387718798573</v>
+        <v>0.8324456631738312</v>
       </c>
       <c r="J5">
-        <v>0.008796250079255804</v>
+        <v>0.002302700220370625</v>
       </c>
       <c r="K5">
         <v>0.8566798373674943</v>
       </c>
       <c r="L5">
-        <v>0.8661642521059694</v>
+        <v>0.8621402850447035</v>
       </c>
       <c r="M5">
-        <v>0.01107113103959569</v>
+        <v>0.006373965440798411</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -719,40 +773,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>13.96617686920821</v>
+        <v>14.49513714816537</v>
       </c>
       <c r="D6">
-        <v>0.02150003230432063</v>
+        <v>0.01987332096301542</v>
       </c>
       <c r="E6">
-        <v>0.2047322548754273</v>
+        <v>0.1967275895461224</v>
       </c>
       <c r="F6">
-        <v>24.18925198261502</v>
+        <v>25.10553536849975</v>
       </c>
       <c r="G6">
-        <v>0.9547937708119657</v>
+        <v>0.9578148707528045</v>
       </c>
       <c r="H6">
         <v>0.8305331942045113</v>
       </c>
       <c r="I6">
-        <v>0.8359238427681156</v>
+        <v>0.8380122104547422</v>
       </c>
       <c r="J6">
-        <v>0.006490587734747268</v>
+        <v>0.009005078066017913</v>
       </c>
       <c r="K6">
         <v>0.8566798373674943</v>
       </c>
       <c r="L6">
-        <v>0.8608786577584859</v>
+        <v>0.8708105294652613</v>
       </c>
       <c r="M6">
-        <v>0.004901271406006525</v>
+        <v>0.01649471772463958</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -760,40 +814,40 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>14.55082357289358</v>
+        <v>14.90953999469957</v>
       </c>
       <c r="D7">
-        <v>0.02188695939810768</v>
+        <v>0.02519401325951733</v>
       </c>
       <c r="E7">
-        <v>0.2151519506573918</v>
+        <v>0.1983441992264328</v>
       </c>
       <c r="F7">
-        <v>25.20183784067272</v>
+        <v>25.82330678671821</v>
       </c>
       <c r="G7">
-        <v>0.9511386957363325</v>
+        <v>0.9500732051899409</v>
       </c>
       <c r="H7">
         <v>0.8305331942045113</v>
       </c>
       <c r="I7">
-        <v>0.8327028629491161</v>
+        <v>0.8307020771951377</v>
       </c>
       <c r="J7">
-        <v>0.002612380528249565</v>
+        <v>0.0002033428546923967</v>
       </c>
       <c r="K7">
         <v>0.8566798373674943</v>
       </c>
       <c r="L7">
-        <v>0.8606237884217683</v>
+        <v>0.8619133396454793</v>
       </c>
       <c r="M7">
-        <v>0.004603763135588044</v>
+        <v>0.006109052705228993</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -801,40 +855,40 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>16.01797336426225</v>
+        <v>13.97310369820133</v>
       </c>
       <c r="D8">
-        <v>0.02381115265884652</v>
+        <v>0.02455844224069879</v>
       </c>
       <c r="E8">
-        <v>0.2043611036310487</v>
+        <v>0.2088979809264863</v>
       </c>
       <c r="F8">
-        <v>27.74318081372388</v>
+        <v>24.20121152749472</v>
       </c>
       <c r="G8">
-        <v>0.9491169824009994</v>
+        <v>0.9498130777369566</v>
       </c>
       <c r="H8">
         <v>0.8305331942045113</v>
       </c>
       <c r="I8">
-        <v>0.8634207289415733</v>
+        <v>0.8403847029257042</v>
       </c>
       <c r="J8">
-        <v>0.03959809790451759</v>
+        <v>0.01186166764909224</v>
       </c>
       <c r="K8">
         <v>0.8566798373674943</v>
       </c>
       <c r="L8">
-        <v>0.8778695364788989</v>
+        <v>0.8614248809577649</v>
       </c>
       <c r="M8">
-        <v>0.02473467704868453</v>
+        <v>0.005538876232749609</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -842,40 +896,40 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>13.88677373839534</v>
+        <v>14.41963511347171</v>
       </c>
       <c r="D9">
-        <v>0.01755671077788934</v>
+        <v>0.02237703584964189</v>
       </c>
       <c r="E9">
-        <v>0.2049131462350555</v>
+        <v>0.2009593755089724</v>
       </c>
       <c r="F9">
-        <v>24.05171837828991</v>
+        <v>24.97472212086972</v>
       </c>
       <c r="G9">
-        <v>0.9592445223806134</v>
+        <v>0.9539640840107021</v>
       </c>
       <c r="H9">
         <v>0.8305331942045113</v>
       </c>
       <c r="I9">
-        <v>0.8441815516240349</v>
+        <v>0.8407822933164411</v>
       </c>
       <c r="J9">
-        <v>0.01643324735815766</v>
+        <v>0.01234038468714831</v>
       </c>
       <c r="K9">
         <v>0.8566798373674943</v>
       </c>
       <c r="L9">
-        <v>0.8732067355692411</v>
+        <v>0.8691386960742697</v>
       </c>
       <c r="M9">
-        <v>0.01929180246909111</v>
+        <v>0.01454319124056948</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -883,40 +937,40 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>14.27737351653631</v>
+        <v>14.85792169486353</v>
       </c>
       <c r="D10">
-        <v>0.01990222700162663</v>
+        <v>0.02048991021828453</v>
       </c>
       <c r="E10">
-        <v>0.2107249532026882</v>
+        <v>0.2144693534636577</v>
       </c>
       <c r="F10">
-        <v>24.72823047627013</v>
+        <v>25.7337734180608</v>
       </c>
       <c r="G10">
-        <v>0.9549042285027749</v>
+        <v>0.9525822005920238</v>
       </c>
       <c r="H10">
         <v>0.8305331942045113</v>
       </c>
       <c r="I10">
-        <v>0.8450733103524251</v>
+        <v>0.8419937550222579</v>
       </c>
       <c r="J10">
-        <v>0.01750696570513394</v>
+        <v>0.01379904005970957</v>
       </c>
       <c r="K10">
         <v>0.8566798373674943</v>
       </c>
       <c r="L10">
-        <v>0.8704912811794304</v>
+        <v>0.8741491184822016</v>
       </c>
       <c r="M10">
-        <v>0.01612206008533774</v>
+        <v>0.02039184343171761</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -927,37 +981,37 @@
         <v>20</v>
       </c>
       <c r="C11">
-        <v>14.37784065144536</v>
+        <v>13.59917378262213</v>
       </c>
       <c r="D11">
-        <v>0.02163497713183102</v>
+        <v>0.0208512555941626</v>
       </c>
       <c r="E11">
-        <v>0.2043564362365518</v>
+        <v>0.2087668677929031</v>
       </c>
       <c r="F11">
-        <v>24.90230261983416</v>
+        <v>23.55352551806041</v>
       </c>
       <c r="G11">
-        <v>0.9541867397530774</v>
+        <v>0.9551091011861824</v>
       </c>
       <c r="H11">
         <v>0.8305331942045113</v>
       </c>
       <c r="I11">
-        <v>0.8493575457102259</v>
+        <v>0.8465542557913764</v>
       </c>
       <c r="J11">
-        <v>0.02266538127202086</v>
+        <v>0.01929009183336756</v>
       </c>
       <c r="K11">
         <v>0.8566798373674943</v>
       </c>
       <c r="L11">
-        <v>0.8754275800602062</v>
+        <v>0.8718620453628055</v>
       </c>
       <c r="M11">
-        <v>0.02188418808865876</v>
+        <v>0.01772214931772514</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -968,37 +1022,37 @@
         <v>21</v>
       </c>
       <c r="C12">
-        <v>13.72353366432195</v>
+        <v>15.01364401938481</v>
       </c>
       <c r="D12">
-        <v>0.0217319804244995</v>
+        <v>0.02244919442254166</v>
       </c>
       <c r="E12">
-        <v>0.2106409259795962</v>
+        <v>0.20034091452527</v>
       </c>
       <c r="F12">
-        <v>23.76891429638014</v>
+        <v>26.00361282156892</v>
       </c>
       <c r="G12">
-        <v>0.9534507822150521</v>
+        <v>0.9532208695257487</v>
       </c>
       <c r="H12">
         <v>0.8305331942045113</v>
       </c>
       <c r="I12">
-        <v>0.8405125793348666</v>
+        <v>0.8344299374690054</v>
       </c>
       <c r="J12">
-        <v>0.01201563670181002</v>
+        <v>0.00469185734138705</v>
       </c>
       <c r="K12">
         <v>0.8566798373674943</v>
       </c>
       <c r="L12">
-        <v>0.8687368738077539</v>
+        <v>0.87517225898979</v>
       </c>
       <c r="M12">
-        <v>0.01407414522245538</v>
+        <v>0.02158615251074586</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1009,37 +1063,37 @@
         <v>22</v>
       </c>
       <c r="C13">
-        <v>13.19257031306449</v>
+        <v>13.88936997590615</v>
       </c>
       <c r="D13">
-        <v>0.02123688459991259</v>
+        <v>0.02238681839371746</v>
       </c>
       <c r="E13">
-        <v>0.2108888504791566</v>
+        <v>0.2127368239744047</v>
       </c>
       <c r="F13">
-        <v>22.84921900816147</v>
+        <v>24.05614343274705</v>
       </c>
       <c r="G13">
-        <v>0.9546440814393914</v>
+        <v>0.9519286485252643</v>
       </c>
       <c r="H13">
         <v>0.8305331942045113</v>
       </c>
       <c r="I13">
-        <v>0.8439160342167965</v>
+        <v>0.8400438152841626</v>
       </c>
       <c r="J13">
-        <v>0.01611355224050175</v>
+        <v>0.01145122331776348</v>
       </c>
       <c r="K13">
         <v>0.8566798373674943</v>
       </c>
       <c r="L13">
-        <v>0.8693946281900901</v>
+        <v>0.8709296799854015</v>
       </c>
       <c r="M13">
-        <v>0.01484194009008924</v>
+        <v>0.01663380179659155</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1050,37 +1104,37 @@
         <v>23</v>
       </c>
       <c r="C14">
-        <v>15.0701726074681</v>
+        <v>14.66160297019964</v>
       </c>
       <c r="D14">
-        <v>0.01638475121110168</v>
+        <v>0.02326103821726664</v>
       </c>
       <c r="E14">
-        <v>0.2126204784465981</v>
+        <v>0.2028670544029265</v>
       </c>
       <c r="F14">
-        <v>26.10143351099171</v>
+        <v>25.39382028859855</v>
       </c>
       <c r="G14">
-        <v>0.9570501609160353</v>
+        <v>0.9520693197863382</v>
       </c>
       <c r="H14">
         <v>0.8305331942045113</v>
       </c>
       <c r="I14">
-        <v>0.8476615501873871</v>
+        <v>0.8431635413241885</v>
       </c>
       <c r="J14">
-        <v>0.02062332499459144</v>
+        <v>0.01520751633747107</v>
       </c>
       <c r="K14">
         <v>0.8566798373674943</v>
       </c>
       <c r="L14">
-        <v>0.8758342800439602</v>
+        <v>0.8618542724413815</v>
       </c>
       <c r="M14">
-        <v>0.02235892785258719</v>
+        <v>0.0060401037215814</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1091,37 +1145,37 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>13.92788203163845</v>
+        <v>14.11435766433111</v>
       </c>
       <c r="D15">
-        <v>0.01937666882596718</v>
+        <v>0.02025859541200383</v>
       </c>
       <c r="E15">
-        <v>0.2024917033855888</v>
+        <v>0.2089343855115164</v>
       </c>
       <c r="F15">
-        <v>24.12294168041031</v>
+        <v>24.44588335163713</v>
       </c>
       <c r="G15">
-        <v>0.9578227571238022</v>
+        <v>0.9551212192095049</v>
       </c>
       <c r="H15">
         <v>0.8305331942045113</v>
       </c>
       <c r="I15">
-        <v>0.8418059339242857</v>
+        <v>0.8380302421247711</v>
       </c>
       <c r="J15">
-        <v>0.01357289485650416</v>
+        <v>0.009026789022491081</v>
       </c>
       <c r="K15">
         <v>0.8566798373674943</v>
       </c>
       <c r="L15">
-        <v>0.8623871455659567</v>
+        <v>0.8670694216377126</v>
       </c>
       <c r="M15">
-        <v>0.006662125043120563</v>
+        <v>0.01212773292545862</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1129,40 +1183,40 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16">
-        <v>14.26522414728236</v>
+        <v>14.12043153646851</v>
       </c>
       <c r="D16">
-        <v>0.02377641073793373</v>
+        <v>0.02240551319811239</v>
       </c>
       <c r="E16">
-        <v>0.2073523814284763</v>
+        <v>0.2116054281026059</v>
       </c>
       <c r="F16">
-        <v>24.70721148953945</v>
+        <v>24.45637915685924</v>
       </c>
       <c r="G16">
-        <v>0.950875507138314</v>
+        <v>0.9518789287439192</v>
       </c>
       <c r="H16">
         <v>0.8305331942045113</v>
       </c>
       <c r="I16">
-        <v>0.8424716007439947</v>
+        <v>0.8459718544622662</v>
       </c>
       <c r="J16">
-        <v>0.01437438819157382</v>
+        <v>0.01858885396211296</v>
       </c>
       <c r="K16">
         <v>0.8566798373674943</v>
       </c>
       <c r="L16">
-        <v>0.8686838800323897</v>
+        <v>0.8727793695549975</v>
       </c>
       <c r="M16">
-        <v>0.01401228573533706</v>
+        <v>0.01879293930504501</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1170,40 +1224,40 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17">
-        <v>13.38424258571819</v>
+        <v>14.94237901252506</v>
       </c>
       <c r="D17">
-        <v>0.02004636237329471</v>
+        <v>0.01918031634900368</v>
       </c>
       <c r="E17">
-        <v>0.2009592397845929</v>
+        <v>0.2115458271018509</v>
       </c>
       <c r="F17">
-        <v>23.18130846840526</v>
+        <v>25.8800879469207</v>
       </c>
       <c r="G17">
-        <v>0.9580821061865453</v>
+        <v>0.9546403969710012</v>
       </c>
       <c r="H17">
         <v>0.8305331942045113</v>
       </c>
       <c r="I17">
-        <v>0.8385963942840614</v>
+        <v>0.8409803733496605</v>
       </c>
       <c r="J17">
-        <v>0.009708462149153536</v>
+        <v>0.01257888211819818</v>
       </c>
       <c r="K17">
         <v>0.8566798373674943</v>
       </c>
       <c r="L17">
-        <v>0.8696827526159603</v>
+        <v>0.8693588215677798</v>
       </c>
       <c r="M17">
-        <v>0.01517826693391413</v>
+        <v>0.0148001431190991</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1211,40 +1265,40 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18">
-        <v>14.72720328681023</v>
+        <v>13.67743445908804</v>
       </c>
       <c r="D18">
-        <v>0.02247396690726244</v>
+        <v>0.02078767259856054</v>
       </c>
       <c r="E18">
-        <v>0.1995080898394706</v>
+        <v>0.2036149427352437</v>
       </c>
       <c r="F18">
-        <v>25.50747422611661</v>
+        <v>23.68912723119427</v>
       </c>
       <c r="G18">
-        <v>0.9537578687813792</v>
+        <v>0.9562656417156613</v>
       </c>
       <c r="H18">
         <v>0.8305331942045113</v>
       </c>
       <c r="I18">
-        <v>0.8441289324054722</v>
+        <v>0.8382666202763119</v>
       </c>
       <c r="J18">
-        <v>0.01636989140931675</v>
+        <v>0.009311399141858167</v>
       </c>
       <c r="K18">
         <v>0.8566798373674943</v>
       </c>
       <c r="L18">
-        <v>0.868770085071581</v>
+        <v>0.864862764271777</v>
       </c>
       <c r="M18">
-        <v>0.01411291263868081</v>
+        <v>0.009551907897620348</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1252,40 +1306,40 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19">
-        <v>14.3380870238199</v>
+        <v>13.46989251526409</v>
       </c>
       <c r="D19">
-        <v>0.0190635812588373</v>
+        <v>0.01946048912614372</v>
       </c>
       <c r="E19">
-        <v>0.2078996581607253</v>
+        <v>0.1978179911453252</v>
       </c>
       <c r="F19">
-        <v>24.83341766289739</v>
+        <v>23.32969143495138</v>
       </c>
       <c r="G19">
-        <v>0.9564131914986452</v>
+        <v>0.959332594239194</v>
       </c>
       <c r="H19">
         <v>0.8305331942045113</v>
       </c>
       <c r="I19">
-        <v>0.8333401902920569</v>
+        <v>0.8408401994454919</v>
       </c>
       <c r="J19">
-        <v>0.003379751835486945</v>
+        <v>0.01241010631833048</v>
       </c>
       <c r="K19">
         <v>0.8566798373674943</v>
       </c>
       <c r="L19">
-        <v>0.8610987084008075</v>
+        <v>0.8619684664994927</v>
       </c>
       <c r="M19">
-        <v>0.005158135910951282</v>
+        <v>0.006173402129142974</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1293,40 +1347,40 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20">
-        <v>14.78018159688398</v>
+        <v>13.76586402562095</v>
       </c>
       <c r="D20">
-        <v>0.01791254086046421</v>
+        <v>0.02125498245776329</v>
       </c>
       <c r="E20">
-        <v>0.2109986726682254</v>
+        <v>0.2010497559579944</v>
       </c>
       <c r="F20">
-        <v>25.59914965016645</v>
+        <v>23.8423187701407</v>
       </c>
       <c r="G20">
-        <v>0.9563269816033851</v>
+        <v>0.9561711369639511</v>
       </c>
       <c r="H20">
         <v>0.8305331942045113</v>
       </c>
       <c r="I20">
-        <v>0.8375629009078456</v>
+        <v>0.8458536532852036</v>
       </c>
       <c r="J20">
-        <v>0.00846408879547233</v>
+        <v>0.01844653433191945</v>
       </c>
       <c r="K20">
         <v>0.8566798373674943</v>
       </c>
       <c r="L20">
-        <v>0.8748666732647333</v>
+        <v>0.870038218509795</v>
       </c>
       <c r="M20">
-        <v>0.02122944314077199</v>
+        <v>0.01559320128666725</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1334,40 +1388,40 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21">
-        <v>13.69595317782271</v>
+        <v>14.10211350926755</v>
       </c>
       <c r="D21">
-        <v>0.0224413494504299</v>
+        <v>0.02251777072397616</v>
       </c>
       <c r="E21">
-        <v>0.1970858392844352</v>
+        <v>0.1959710159395474</v>
       </c>
       <c r="F21">
-        <v>23.72125742672854</v>
+        <v>24.42478054345039</v>
       </c>
       <c r="G21">
-        <v>0.9556539171398857</v>
+        <v>0.95528956032125</v>
       </c>
       <c r="H21">
         <v>0.8305331942045113</v>
       </c>
       <c r="I21">
-        <v>0.8363240099529845</v>
+        <v>0.8352571033307269</v>
       </c>
       <c r="J21">
-        <v>0.006972407350942364</v>
+        <v>0.005687802918870867</v>
       </c>
       <c r="K21">
         <v>0.8566798373674943</v>
       </c>
       <c r="L21">
-        <v>0.8686392472572797</v>
+        <v>0.8678334394269771</v>
       </c>
       <c r="M21">
-        <v>0.01396018602064414</v>
+        <v>0.01301956877350689</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1375,40 +1429,40 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22">
-        <v>14.19636903930732</v>
+        <v>14.66032392387194</v>
       </c>
       <c r="D22">
-        <v>0.01760515319541675</v>
+        <v>0.01875895782382112</v>
       </c>
       <c r="E22">
-        <v>0.1985421000894003</v>
+        <v>0.2073701486642589</v>
       </c>
       <c r="F22">
-        <v>24.58802458095575</v>
+        <v>25.39157219199907</v>
       </c>
       <c r="G22">
-        <v>0.960228224169264</v>
+        <v>0.9564421833227937</v>
       </c>
       <c r="H22">
         <v>0.8305331942045113</v>
       </c>
       <c r="I22">
-        <v>0.8331445793985282</v>
+        <v>0.8509238068048006</v>
       </c>
       <c r="J22">
-        <v>0.003144227361698675</v>
+        <v>0.02455123135664616</v>
       </c>
       <c r="K22">
         <v>0.8566798373674943</v>
       </c>
       <c r="L22">
-        <v>0.8624686302432595</v>
+        <v>0.877567831333405</v>
       </c>
       <c r="M22">
-        <v>0.006757241881113541</v>
+        <v>0.02438249746847987</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1416,40 +1470,40 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23">
-        <v>14.42163603278877</v>
+        <v>14.3947143675402</v>
       </c>
       <c r="D23">
-        <v>0.02074362999377977</v>
+        <v>0.02309991194440809</v>
       </c>
       <c r="E23">
-        <v>0.2104381321900189</v>
+        <v>0.2056268991486042</v>
       </c>
       <c r="F23">
-        <v>24.97811127929874</v>
+        <v>24.93151798711061</v>
       </c>
       <c r="G23">
-        <v>0.9538091624240973</v>
+        <v>0.9520073513640449</v>
       </c>
       <c r="H23">
         <v>0.8305331942045113</v>
       </c>
       <c r="I23">
-        <v>0.8426508162254081</v>
+        <v>0.8349977892381517</v>
       </c>
       <c r="J23">
-        <v>0.01459017183834903</v>
+        <v>0.005375576876149537</v>
       </c>
       <c r="K23">
         <v>0.8566798373674943</v>
       </c>
       <c r="L23">
-        <v>0.873988692287135</v>
+        <v>0.8650205535801767</v>
       </c>
       <c r="M23">
-        <v>0.0202045783788135</v>
+        <v>0.009736094920026042</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1457,40 +1511,40 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24">
-        <v>15.35125661991043</v>
+        <v>14.524244825464</v>
       </c>
       <c r="D24">
-        <v>0.02586906026469911</v>
+        <v>0.02010023859576943</v>
       </c>
       <c r="E24">
-        <v>0.2072585058478998</v>
+        <v>0.2122825201021538</v>
       </c>
       <c r="F24">
-        <v>26.58833605426461</v>
+        <v>25.15582627070954</v>
       </c>
       <c r="G24">
-        <v>0.9464837743951012</v>
+        <v>0.9539925667743847</v>
       </c>
       <c r="H24">
         <v>0.8305331942045113</v>
       </c>
       <c r="I24">
-        <v>0.8598928838379858</v>
+        <v>0.8411090459165464</v>
       </c>
       <c r="J24">
-        <v>0.03535041084251342</v>
+        <v>0.01273380978127518</v>
       </c>
       <c r="K24">
         <v>0.8566798373674943</v>
       </c>
       <c r="L24">
-        <v>0.8728792550459286</v>
+        <v>0.8652936142303648</v>
       </c>
       <c r="M24">
-        <v>0.01890953536179129</v>
+        <v>0.01005483786024412</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1498,40 +1552,40 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C25">
-        <v>13.84562852398516</v>
+        <v>14.53507133645294</v>
       </c>
       <c r="D25">
-        <v>0.02088359925430661</v>
+        <v>0.02221422888410251</v>
       </c>
       <c r="E25">
-        <v>0.2011775641867217</v>
+        <v>0.2111081248793957</v>
       </c>
       <c r="F25">
-        <v>23.98047912647966</v>
+        <v>25.17458710992046</v>
       </c>
       <c r="G25">
-        <v>0.9564896075881092</v>
+        <v>0.9517029574285427</v>
       </c>
       <c r="H25">
         <v>0.8305331942045113</v>
       </c>
       <c r="I25">
-        <v>0.8359401320073027</v>
+        <v>0.8460067120584497</v>
       </c>
       <c r="J25">
-        <v>0.006510200724692437</v>
+        <v>0.01863082410421773</v>
       </c>
       <c r="K25">
         <v>0.8566798373674943</v>
       </c>
       <c r="L25">
-        <v>0.8661838087819154</v>
+        <v>0.8690527123702526</v>
       </c>
       <c r="M25">
-        <v>0.01109395949322907</v>
+        <v>0.01444282270116116</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1539,40 +1593,40 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C26">
-        <v>13.98303486306176</v>
+        <v>14.11485799363989</v>
       </c>
       <c r="D26">
-        <v>0.0225243942429423</v>
+        <v>0.01955891295117575</v>
       </c>
       <c r="E26">
-        <v>0.1978604158388224</v>
+        <v>0.204703539792901</v>
       </c>
       <c r="F26">
-        <v>24.21850812606569</v>
+        <v>24.44678634200373</v>
       </c>
       <c r="G26">
-        <v>0.9550195391990016</v>
+        <v>0.956884842150962</v>
       </c>
       <c r="H26">
         <v>0.8305331942045113</v>
       </c>
       <c r="I26">
-        <v>0.8391464165975572</v>
+        <v>0.8314579319455953</v>
       </c>
       <c r="J26">
-        <v>0.01037071420281478</v>
+        <v>0.001113426588529846</v>
       </c>
       <c r="K26">
         <v>0.8566798373674943</v>
       </c>
       <c r="L26">
-        <v>0.8630899702509721</v>
+        <v>0.8613865444695308</v>
       </c>
       <c r="M26">
-        <v>0.007482530350166297</v>
+        <v>0.005494126156277689</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1580,40 +1634,40 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C27">
-        <v>14.21424845304317</v>
+        <v>13.20135859516718</v>
       </c>
       <c r="D27">
-        <v>0.01991312393311727</v>
+        <v>0.02095508717301163</v>
       </c>
       <c r="E27">
-        <v>0.1991073750490557</v>
+        <v>0.2062280068260026</v>
       </c>
       <c r="F27">
-        <v>24.61898732635479</v>
+        <v>22.8644841876677</v>
       </c>
       <c r="G27">
-        <v>0.9576113939805991</v>
+        <v>0.9560500026648308</v>
       </c>
       <c r="H27">
         <v>0.8305331942045113</v>
       </c>
       <c r="I27">
-        <v>0.8442753156331009</v>
+        <v>0.8368446367256889</v>
       </c>
       <c r="J27">
-        <v>0.0165461435189858</v>
+        <v>0.007599265827325151</v>
       </c>
       <c r="K27">
         <v>0.8566798373674943</v>
       </c>
       <c r="L27">
-        <v>0.8729444522170001</v>
+        <v>0.8680676084416795</v>
       </c>
       <c r="M27">
-        <v>0.01898563983889899</v>
+        <v>0.01329291361540488</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -1621,40 +1675,40 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28">
-        <v>13.46604445963164</v>
+        <v>14.00944728863614</v>
       </c>
       <c r="D28">
-        <v>0.019245774525832</v>
+        <v>0.0230771304572704</v>
       </c>
       <c r="E28">
-        <v>0.1994204209148302</v>
+        <v>0.2119809145174359</v>
       </c>
       <c r="F28">
-        <v>23.32301269695261</v>
+        <v>24.26413756013499</v>
       </c>
       <c r="G28">
-        <v>0.9592215331948483</v>
+        <v>0.9510604696987351</v>
       </c>
       <c r="H28">
         <v>0.8305331942045113</v>
       </c>
       <c r="I28">
-        <v>0.8329416384678092</v>
+        <v>0.8333274768543103</v>
       </c>
       <c r="J28">
-        <v>0.002899877187455117</v>
+        <v>0.003364444274229582</v>
       </c>
       <c r="K28">
         <v>0.8566798373674943</v>
       </c>
       <c r="L28">
-        <v>0.8667747507598222</v>
+        <v>0.8562385170549937</v>
       </c>
       <c r="M28">
-        <v>0.01178376442633313</v>
+        <v>0.0005151519777292761</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1662,40 +1716,40 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29">
-        <v>15.0965454764834</v>
+        <v>14.6648863918671</v>
       </c>
       <c r="D29">
-        <v>0.01800059733112618</v>
+        <v>0.01716168436134764</v>
       </c>
       <c r="E29">
-        <v>0.2074003787346325</v>
+        <v>0.2013464758881534</v>
       </c>
       <c r="F29">
-        <v>26.14715504662004</v>
+        <v>25.3995244784689</v>
       </c>
       <c r="G29">
-        <v>0.9566447979404461</v>
+        <v>0.9594366321252495</v>
       </c>
       <c r="H29">
         <v>0.8305331942045113</v>
       </c>
       <c r="I29">
-        <v>0.8340192597171786</v>
+        <v>0.8379364282362395</v>
       </c>
       <c r="J29">
-        <v>0.00419738252124438</v>
+        <v>0.008913832804502184</v>
       </c>
       <c r="K29">
         <v>0.8566798373674943</v>
       </c>
       <c r="L29">
-        <v>0.8630984336537355</v>
+        <v>0.8577295394288736</v>
       </c>
       <c r="M29">
-        <v>0.00749240965675696</v>
+        <v>0.00122531430715701</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -1703,40 +1757,40 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30">
-        <v>14.93600564990906</v>
+        <v>13.89130508475239</v>
       </c>
       <c r="D30">
-        <v>0.01871090577916044</v>
+        <v>0.02182124811138559</v>
       </c>
       <c r="E30">
-        <v>0.2090929384838661</v>
+        <v>0.2036116324274554</v>
       </c>
       <c r="F30">
-        <v>25.86906887322052</v>
+        <v>24.05957474705806</v>
       </c>
       <c r="G30">
-        <v>0.9557279675885546</v>
+        <v>0.9547445783905428</v>
       </c>
       <c r="H30">
         <v>0.8305331942045113</v>
       </c>
       <c r="I30">
-        <v>0.8424717708171592</v>
+        <v>0.8465097406603371</v>
       </c>
       <c r="J30">
-        <v>0.01437459296745229</v>
+        <v>0.01923649357703061</v>
       </c>
       <c r="K30">
         <v>0.8566798373674943</v>
       </c>
       <c r="L30">
-        <v>0.8692755715592919</v>
+        <v>0.8710634827407766</v>
       </c>
       <c r="M30">
-        <v>0.01470296561490608</v>
+        <v>0.01678998938212674</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1744,40 +1798,40 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31">
-        <v>14.81335506401023</v>
+        <v>14.85290343570587</v>
       </c>
       <c r="D31">
-        <v>0.01897692065230458</v>
+        <v>0.022205537385087</v>
       </c>
       <c r="E31">
-        <v>0.2039800834288993</v>
+        <v>0.2085744035693952</v>
       </c>
       <c r="F31">
-        <v>25.65666573737436</v>
+        <v>25.72512828040893</v>
       </c>
       <c r="G31">
-        <v>0.9567769664331722</v>
+        <v>0.9518819715612702</v>
       </c>
       <c r="H31">
         <v>0.8305331942045113</v>
       </c>
       <c r="I31">
-        <v>0.8525829469646994</v>
+        <v>0.8414464039999884</v>
       </c>
       <c r="J31">
-        <v>0.02654891208930838</v>
+        <v>0.01314000436301619</v>
       </c>
       <c r="K31">
         <v>0.8566798373674943</v>
       </c>
       <c r="L31">
-        <v>0.8679911113999897</v>
+        <v>0.8708178933077839</v>
       </c>
       <c r="M31">
-        <v>0.01320361883064044</v>
+        <v>0.01650331351760848</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -1785,40 +1839,40 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32">
-        <v>13.73884603594896</v>
+        <v>15.55182431012915</v>
       </c>
       <c r="D32">
-        <v>0.02331513586814974</v>
+        <v>0.02480963043454181</v>
       </c>
       <c r="E32">
-        <v>0.2049084959967496</v>
+        <v>0.2149192323644518</v>
       </c>
       <c r="F32">
-        <v>23.79548570866413</v>
+        <v>26.93568102582833</v>
       </c>
       <c r="G32">
-        <v>0.9527180793573171</v>
+        <v>0.9459431512327585</v>
       </c>
       <c r="H32">
         <v>0.8305331942045113</v>
       </c>
       <c r="I32">
-        <v>0.8416740722488228</v>
+        <v>0.8469888928514077</v>
       </c>
       <c r="J32">
-        <v>0.01341412736065571</v>
+        <v>0.01981341475780228</v>
       </c>
       <c r="K32">
         <v>0.8566798373674943</v>
       </c>
       <c r="L32">
-        <v>0.8656086119961505</v>
+        <v>0.8615437633787786</v>
       </c>
       <c r="M32">
-        <v>0.01042253387927693</v>
+        <v>0.005677647353334133</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -1826,40 +1880,40 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33">
-        <v>14.16712890194452</v>
+        <v>14.87519061135661</v>
       </c>
       <c r="D33">
-        <v>0.02568063869611423</v>
+        <v>0.02346391014792033</v>
       </c>
       <c r="E33">
-        <v>0.2022726081988335</v>
+        <v>0.20388946621322</v>
       </c>
       <c r="F33">
-        <v>24.53733991837142</v>
+        <v>25.76376846858902</v>
       </c>
       <c r="G33">
-        <v>0.9494686529639745</v>
+        <v>0.9512840244984146</v>
       </c>
       <c r="H33">
         <v>0.8305331942045113</v>
       </c>
       <c r="I33">
-        <v>0.8441093989854332</v>
+        <v>0.8463098258521095</v>
       </c>
       <c r="J33">
-        <v>0.01634637227705904</v>
+        <v>0.01899578699284748</v>
       </c>
       <c r="K33">
         <v>0.8566798373674943</v>
       </c>
       <c r="L33">
-        <v>0.8674665841852508</v>
+        <v>0.8672382268502032</v>
       </c>
       <c r="M33">
-        <v>0.0125913396665238</v>
+        <v>0.01232477878218073</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1867,40 +1921,40 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34">
-        <v>13.9529975257797</v>
+        <v>13.63836111197879</v>
       </c>
       <c r="D34">
-        <v>0.01764304187228453</v>
+        <v>0.02165476085308455</v>
       </c>
       <c r="E34">
-        <v>0.19879789416476</v>
+        <v>0.2086030104552899</v>
       </c>
       <c r="F34">
-        <v>24.16647653224589</v>
+        <v>23.62140337316069</v>
       </c>
       <c r="G34">
-        <v>0.9604427832343906</v>
+        <v>0.9541248802119645</v>
       </c>
       <c r="H34">
         <v>0.8305331942045113</v>
       </c>
       <c r="I34">
-        <v>0.8454086749833487</v>
+        <v>0.8381822866308851</v>
       </c>
       <c r="J34">
-        <v>0.01791076007875301</v>
+        <v>0.009209857570714113</v>
       </c>
       <c r="K34">
         <v>0.8566798373674943</v>
       </c>
       <c r="L34">
-        <v>0.872673001696681</v>
+        <v>0.869871807420329</v>
       </c>
       <c r="M34">
-        <v>0.01866877639881475</v>
+        <v>0.01539895008311682</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -1908,40 +1962,40 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C35">
-        <v>13.71966471029614</v>
+        <v>14.39677581203059</v>
       </c>
       <c r="D35">
-        <v>0.01787799550175513</v>
+        <v>0.02211775059283683</v>
       </c>
       <c r="E35">
-        <v>0.2007927176638888</v>
+        <v>0.2004677850518101</v>
       </c>
       <c r="F35">
-        <v>23.76230127640513</v>
+        <v>24.93513153801024</v>
       </c>
       <c r="G35">
-        <v>0.9600542717956072</v>
+        <v>0.9544321474598245</v>
       </c>
       <c r="H35">
         <v>0.8305331942045113</v>
       </c>
       <c r="I35">
-        <v>0.8407866790648645</v>
+        <v>0.8386052019421659</v>
       </c>
       <c r="J35">
-        <v>0.012345665329095</v>
+        <v>0.009719066972857121</v>
       </c>
       <c r="K35">
         <v>0.8566798373674943</v>
       </c>
       <c r="L35">
-        <v>0.8679796230215675</v>
+        <v>0.8607121841832319</v>
       </c>
       <c r="M35">
-        <v>0.01319020847834646</v>
+        <v>0.004706947262968946</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -1949,40 +2003,40 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C36">
-        <v>14.8912106730875</v>
+        <v>14.11386047806839</v>
       </c>
       <c r="D36">
-        <v>0.01981920778933351</v>
+        <v>0.02249558166508224</v>
       </c>
       <c r="E36">
-        <v>0.2055105714835023</v>
+        <v>0.2055401660766999</v>
       </c>
       <c r="F36">
-        <v>25.79150710088176</v>
+        <v>24.44504898690277</v>
       </c>
       <c r="G36">
-        <v>0.9553934929509277</v>
+        <v>0.9531740056519368</v>
       </c>
       <c r="H36">
         <v>0.8305331942045113</v>
       </c>
       <c r="I36">
-        <v>0.8410621355452648</v>
+        <v>0.8375466376434409</v>
       </c>
       <c r="J36">
-        <v>0.01267732754599665</v>
+        <v>0.008444507080354727</v>
       </c>
       <c r="K36">
         <v>0.8566798373674943</v>
       </c>
       <c r="L36">
-        <v>0.8645073248801791</v>
+        <v>0.8698663231135531</v>
       </c>
       <c r="M36">
-        <v>0.009137004480854857</v>
+        <v>0.01539254826701619</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -1990,40 +2044,40 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C37">
-        <v>13.81317055899715</v>
+        <v>14.46150984987053</v>
       </c>
       <c r="D37">
-        <v>0.01890011437713879</v>
+        <v>0.02021240231891561</v>
       </c>
       <c r="E37">
-        <v>0.2051307832063063</v>
+        <v>0.2041802047401146</v>
       </c>
       <c r="F37">
-        <v>23.92422635788445</v>
+        <v>25.04722945390352</v>
       </c>
       <c r="G37">
-        <v>0.957890340474377</v>
+        <v>0.955815487921481</v>
       </c>
       <c r="H37">
         <v>0.8305331942045113</v>
       </c>
       <c r="I37">
-        <v>0.8435111772602201</v>
+        <v>0.839111772831552</v>
       </c>
       <c r="J37">
-        <v>0.0156260859244032</v>
+        <v>0.01032900152203706</v>
       </c>
       <c r="K37">
         <v>0.8566798373674943</v>
       </c>
       <c r="L37">
-        <v>0.8674184701188921</v>
+        <v>0.8585193000921645</v>
       </c>
       <c r="M37">
-        <v>0.01253517625020413</v>
+        <v>0.002147199740713738</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2031,40 +2085,40 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C38">
-        <v>14.32525508932702</v>
+        <v>14.25578043798047</v>
       </c>
       <c r="D38">
-        <v>0.02029774916779081</v>
+        <v>0.02092886061616778</v>
       </c>
       <c r="E38">
-        <v>0.2049205229917712</v>
+        <v>0.2086215600930055</v>
       </c>
       <c r="F38">
-        <v>24.81121511944757</v>
+        <v>24.69084580801508</v>
       </c>
       <c r="G38">
-        <v>0.9557259559591819</v>
+        <v>0.9542253865096662</v>
       </c>
       <c r="H38">
         <v>0.8305331942045113</v>
       </c>
       <c r="I38">
-        <v>0.8420217301513903</v>
+        <v>0.8374408807185464</v>
       </c>
       <c r="J38">
-        <v>0.01383272339630291</v>
+        <v>0.00831717089965474</v>
       </c>
       <c r="K38">
         <v>0.8566798373674943</v>
       </c>
       <c r="L38">
-        <v>0.8592132280638389</v>
+        <v>0.8694978659204059</v>
       </c>
       <c r="M38">
-        <v>0.002957219938932514</v>
+        <v>0.01496244920657911</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2072,40 +2126,40 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C39">
-        <v>14.19936653074449</v>
+        <v>13.93541782448347</v>
       </c>
       <c r="D39">
-        <v>0.01808704388418069</v>
+        <v>0.01995113732065895</v>
       </c>
       <c r="E39">
-        <v>0.1926432115923575</v>
+        <v>0.2045966812598946</v>
       </c>
       <c r="F39">
-        <v>24.59326312377334</v>
+        <v>24.13597630051315</v>
       </c>
       <c r="G39">
-        <v>0.961012612868307</v>
+        <v>0.956694150775777</v>
       </c>
       <c r="H39">
         <v>0.8305331942045113</v>
       </c>
       <c r="I39">
-        <v>0.8382825729930747</v>
+        <v>0.8276925912466725</v>
       </c>
       <c r="J39">
-        <v>0.009330606943393518</v>
+        <v>0.003420216046343069</v>
       </c>
       <c r="K39">
         <v>0.8566798373674943</v>
       </c>
       <c r="L39">
-        <v>0.8685832684152593</v>
+        <v>0.8633427103767827</v>
       </c>
       <c r="M39">
-        <v>0.0138948420734907</v>
+        <v>0.007777553198593788</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2113,40 +2167,40 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C40">
-        <v>13.55260790269278</v>
+        <v>14.08959486622078</v>
       </c>
       <c r="D40">
-        <v>0.01705289621497049</v>
+        <v>0.01822274400990452</v>
       </c>
       <c r="E40">
-        <v>0.201295928935244</v>
+        <v>0.2063205929052859</v>
       </c>
       <c r="F40">
-        <v>23.47293616146299</v>
+        <v>24.40301518721092</v>
       </c>
       <c r="G40">
-        <v>0.9609695385319478</v>
+        <v>0.9579883050993855</v>
       </c>
       <c r="H40">
         <v>0.8305331942045113</v>
       </c>
       <c r="I40">
-        <v>0.8475448221930681</v>
+        <v>0.8416022731535643</v>
       </c>
       <c r="J40">
-        <v>0.02048277914388556</v>
+        <v>0.0133276779619326</v>
       </c>
       <c r="K40">
         <v>0.8566798373674943</v>
       </c>
       <c r="L40">
-        <v>0.8727857132870295</v>
+        <v>0.8618651167624969</v>
       </c>
       <c r="M40">
-        <v>0.01880034432586528</v>
+        <v>0.006052762267566031</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2154,40 +2208,1475 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>13.43109083344717</v>
+      </c>
+      <c r="D41">
+        <v>0.01685776868659789</v>
+      </c>
+      <c r="E41">
+        <v>0.1973032028369733</v>
+      </c>
+      <c r="F41">
+        <v>23.26248890791161</v>
+      </c>
+      <c r="G41">
+        <v>0.9621880358127899</v>
+      </c>
+      <c r="H41">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I41">
+        <v>0.8373771753235953</v>
+      </c>
+      <c r="J41">
+        <v>0.008240466686752018</v>
+      </c>
+      <c r="K41">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L41">
+        <v>0.8703232453769209</v>
+      </c>
+      <c r="M41">
+        <v>0.01592591235875423</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>14.10620597740402</v>
+      </c>
+      <c r="D42">
+        <v>0.01682224292691021</v>
+      </c>
+      <c r="E42">
+        <v>0.2109991495797034</v>
+      </c>
+      <c r="F42">
+        <v>24.43174855801087</v>
+      </c>
+      <c r="G42">
+        <v>0.9582848941917265</v>
+      </c>
+      <c r="H42">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I42">
+        <v>0.8505526392025969</v>
+      </c>
+      <c r="J42">
+        <v>0.02410432856601274</v>
+      </c>
+      <c r="K42">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L42">
+        <v>0.8760416189246587</v>
+      </c>
+      <c r="M42">
+        <v>0.02260095395341804</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43">
+        <v>14.21177606553885</v>
+      </c>
+      <c r="D43">
+        <v>0.01975199667308179</v>
+      </c>
+      <c r="E43">
+        <v>0.1990584811177238</v>
+      </c>
+      <c r="F43">
+        <v>24.61470540938464</v>
+      </c>
+      <c r="G43">
+        <v>0.9578076106185041</v>
+      </c>
+      <c r="H43">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I43">
+        <v>0.8374180118969921</v>
+      </c>
+      <c r="J43">
+        <v>0.008289635791228114</v>
+      </c>
+      <c r="K43">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L43">
+        <v>0.8658138748966395</v>
+      </c>
+      <c r="M43">
+        <v>0.0106621366941626</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <v>14.51498722785136</v>
+      </c>
+      <c r="D44">
+        <v>0.02110966685354456</v>
+      </c>
+      <c r="E44">
+        <v>0.2046190993036411</v>
+      </c>
+      <c r="F44">
+        <v>25.13985378000894</v>
+      </c>
+      <c r="G44">
+        <v>0.9545888399172887</v>
+      </c>
+      <c r="H44">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I44">
+        <v>0.8513255364220237</v>
+      </c>
+      <c r="J44">
+        <v>0.02503493221294709</v>
+      </c>
+      <c r="K44">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L44">
+        <v>0.8779837751696942</v>
+      </c>
+      <c r="M44">
+        <v>0.02486802755585457</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45">
+        <v>13.61565595587223</v>
+      </c>
+      <c r="D45">
+        <v>0.02470622706807319</v>
+      </c>
+      <c r="E45">
+        <v>0.208829750494307</v>
+      </c>
+      <c r="F45">
+        <v>23.58207033031004</v>
+      </c>
+      <c r="G45">
+        <v>0.9500659994905947</v>
+      </c>
+      <c r="H45">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I45">
+        <v>0.840761933859946</v>
+      </c>
+      <c r="J45">
+        <v>0.01231587096916918</v>
+      </c>
+      <c r="K45">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L45">
+        <v>0.8603039183915779</v>
+      </c>
+      <c r="M45">
+        <v>0.004230379735818371</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="C41">
-        <v>13.45861173101778</v>
-      </c>
-      <c r="D41">
-        <v>0.01774206821313178</v>
-      </c>
-      <c r="E41">
-        <v>0.2042507095113794</v>
-      </c>
-      <c r="F41">
-        <v>23.31009772706984</v>
-      </c>
-      <c r="G41">
-        <v>0.9597361710434988</v>
-      </c>
-      <c r="H41">
-        <v>0.8305331942045113</v>
-      </c>
-      <c r="I41">
-        <v>0.8409504480583586</v>
-      </c>
-      <c r="J41">
-        <v>0.01254285069704527</v>
-      </c>
-      <c r="K41">
-        <v>0.8566798373674943</v>
-      </c>
-      <c r="L41">
-        <v>0.8753438444061845</v>
-      </c>
-      <c r="M41">
-        <v>0.02178644369178004</v>
+      <c r="B46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46">
+        <v>13.85853668219642</v>
+      </c>
+      <c r="D46">
+        <v>0.01939972707295026</v>
+      </c>
+      <c r="E46">
+        <v>0.2066803638171457</v>
+      </c>
+      <c r="F46">
+        <v>24.00279199995601</v>
+      </c>
+      <c r="G46">
+        <v>0.9569344211338043</v>
+      </c>
+      <c r="H46">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I46">
+        <v>0.8379314013755149</v>
+      </c>
+      <c r="J46">
+        <v>0.008907780233985264</v>
+      </c>
+      <c r="K46">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L46">
+        <v>0.8635755701230629</v>
+      </c>
+      <c r="M46">
+        <v>0.008049369735090944</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>14.23273783878163</v>
+      </c>
+      <c r="D47">
+        <v>0.02458837086356262</v>
+      </c>
+      <c r="E47">
+        <v>0.2134181321662829</v>
+      </c>
+      <c r="F47">
+        <v>24.65088897535626</v>
+      </c>
+      <c r="G47">
+        <v>0.9483830339554092</v>
+      </c>
+      <c r="H47">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I47">
+        <v>0.8502002040227719</v>
+      </c>
+      <c r="J47">
+        <v>0.02367998046977242</v>
+      </c>
+      <c r="K47">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L47">
+        <v>0.8728279554166111</v>
+      </c>
+      <c r="M47">
+        <v>0.01884965344665818</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48">
+        <v>13.55178083986354</v>
+      </c>
+      <c r="D48">
+        <v>0.02111920272060484</v>
+      </c>
+      <c r="E48">
+        <v>0.2007893892572737</v>
+      </c>
+      <c r="F48">
+        <v>23.47150462572682</v>
+      </c>
+      <c r="G48">
+        <v>0.9566569450506129</v>
+      </c>
+      <c r="H48">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I48">
+        <v>0.8365699374067413</v>
+      </c>
+      <c r="J48">
+        <v>0.007268515267486742</v>
+      </c>
+      <c r="K48">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L48">
+        <v>0.865486165326505</v>
+      </c>
+      <c r="M48">
+        <v>0.01027960222114229</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49">
+        <v>15.07635875795822</v>
+      </c>
+      <c r="D49">
+        <v>0.0244062144987017</v>
+      </c>
+      <c r="E49">
+        <v>0.2148483373982036</v>
+      </c>
+      <c r="F49">
+        <v>26.11212409446231</v>
+      </c>
+      <c r="G49">
+        <v>0.9471830033355314</v>
+      </c>
+      <c r="H49">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I49">
+        <v>0.8533881807957938</v>
+      </c>
+      <c r="J49">
+        <v>0.02751845049754225</v>
+      </c>
+      <c r="K49">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L49">
+        <v>0.8813043949647331</v>
+      </c>
+      <c r="M49">
+        <v>0.02874417784000615</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50">
+        <v>14.86818668252153</v>
+      </c>
+      <c r="D50">
+        <v>0.02073618888279957</v>
+      </c>
+      <c r="E50">
+        <v>0.2109268069200725</v>
+      </c>
+      <c r="F50">
+        <v>25.75158258382434</v>
+      </c>
+      <c r="G50">
+        <v>0.9531139855583235</v>
+      </c>
+      <c r="H50">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I50">
+        <v>0.8487929401970007</v>
+      </c>
+      <c r="J50">
+        <v>0.02198557037804929</v>
+      </c>
+      <c r="K50">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L50">
+        <v>0.872274399753027</v>
+      </c>
+      <c r="M50">
+        <v>0.01820348945465261</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51">
+        <v>14.24925391799826</v>
+      </c>
+      <c r="D51">
+        <v>0.01873612076802668</v>
+      </c>
+      <c r="E51">
+        <v>0.1925850017085324</v>
+      </c>
+      <c r="F51">
+        <v>24.67967324811373</v>
+      </c>
+      <c r="G51">
+        <v>0.9602794342731412</v>
+      </c>
+      <c r="H51">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I51">
+        <v>0.8369040246736025</v>
+      </c>
+      <c r="J51">
+        <v>0.007670771636277778</v>
+      </c>
+      <c r="K51">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L51">
+        <v>0.8673400388265529</v>
+      </c>
+      <c r="M51">
+        <v>0.01244362362001709</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52">
+        <v>13.96124443486826</v>
+      </c>
+      <c r="D52">
+        <v>0.02273146293175461</v>
+      </c>
+      <c r="E52">
+        <v>0.2019777596346334</v>
+      </c>
+      <c r="F52">
+        <v>24.1807304847398</v>
+      </c>
+      <c r="G52">
+        <v>0.953867489792272</v>
+      </c>
+      <c r="H52">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I52">
+        <v>0.8452558403880553</v>
+      </c>
+      <c r="J52">
+        <v>0.01772674022697605</v>
+      </c>
+      <c r="K52">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L52">
+        <v>0.8726875800303514</v>
+      </c>
+      <c r="M52">
+        <v>0.0186857936473065</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53">
+        <v>14.07707741717936</v>
+      </c>
+      <c r="D53">
+        <v>0.02070188394352684</v>
+      </c>
+      <c r="E53">
+        <v>0.1985064035219516</v>
+      </c>
+      <c r="F53">
+        <v>24.3813964421143</v>
+      </c>
+      <c r="G53">
+        <v>0.9570052578144018</v>
+      </c>
+      <c r="H53">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I53">
+        <v>0.8283210172955691</v>
+      </c>
+      <c r="J53">
+        <v>0.002663562304768684</v>
+      </c>
+      <c r="K53">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L53">
+        <v>0.8614416923324251</v>
+      </c>
+      <c r="M53">
+        <v>0.005558500103800201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54">
+        <v>14.70613653959827</v>
+      </c>
+      <c r="D54">
+        <v>0.01988979298089617</v>
+      </c>
+      <c r="E54">
+        <v>0.1990077649737655</v>
+      </c>
+      <c r="F54">
+        <v>25.47099048073197</v>
+      </c>
+      <c r="G54">
+        <v>0.9570182836102491</v>
+      </c>
+      <c r="H54">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I54">
+        <v>0.8371531917021064</v>
+      </c>
+      <c r="J54">
+        <v>0.007970780149173672</v>
+      </c>
+      <c r="K54">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L54">
+        <v>0.864419243417174</v>
+      </c>
+      <c r="M54">
+        <v>0.009034187233193509</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>14.10021100882039</v>
+      </c>
+      <c r="D55">
+        <v>0.02152011319114715</v>
+      </c>
+      <c r="E55">
+        <v>0.2150755082290759</v>
+      </c>
+      <c r="F55">
+        <v>24.42132533033919</v>
+      </c>
+      <c r="G55">
+        <v>0.952193283412479</v>
+      </c>
+      <c r="H55">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I55">
+        <v>0.8383413447258121</v>
+      </c>
+      <c r="J55">
+        <v>0.00940137080105447</v>
+      </c>
+      <c r="K55">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L55">
+        <v>0.8636522335492979</v>
+      </c>
+      <c r="M55">
+        <v>0.008138858740073954</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56">
+        <v>13.82288033299668</v>
+      </c>
+      <c r="D56">
+        <v>0.01766371068200422</v>
+      </c>
+      <c r="E56">
+        <v>0.2228838774279333</v>
+      </c>
+      <c r="F56">
+        <v>23.94088705272939</v>
+      </c>
+      <c r="G56">
+        <v>0.9549567337858029</v>
+      </c>
+      <c r="H56">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I56">
+        <v>0.8372117967402498</v>
+      </c>
+      <c r="J56">
+        <v>0.008041343298909666</v>
+      </c>
+      <c r="K56">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L56">
+        <v>0.8661496843108176</v>
+      </c>
+      <c r="M56">
+        <v>0.01105412609268751</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57">
+        <v>14.43398277484873</v>
+      </c>
+      <c r="D57">
+        <v>0.02001350559100407</v>
+      </c>
+      <c r="E57">
+        <v>0.2052919306225131</v>
+      </c>
+      <c r="F57">
+        <v>24.99954061411335</v>
+      </c>
+      <c r="G57">
+        <v>0.9558272651872618</v>
+      </c>
+      <c r="H57">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I57">
+        <v>0.8329472191054043</v>
+      </c>
+      <c r="J57">
+        <v>0.002906596530684237</v>
+      </c>
+      <c r="K57">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L57">
+        <v>0.8590529495708403</v>
+      </c>
+      <c r="M57">
+        <v>0.002770127298242939</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58">
+        <v>13.76899079743012</v>
+      </c>
+      <c r="D58">
+        <v>0.01780358254511211</v>
+      </c>
+      <c r="E58">
+        <v>0.208975901658605</v>
+      </c>
+      <c r="F58">
+        <v>23.84766937971336</v>
+      </c>
+      <c r="G58">
+        <v>0.9582106761135649</v>
+      </c>
+      <c r="H58">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I58">
+        <v>0.8418578077089213</v>
+      </c>
+      <c r="J58">
+        <v>0.01363535326875973</v>
+      </c>
+      <c r="K58">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L58">
+        <v>0.8697262118639197</v>
+      </c>
+      <c r="M58">
+        <v>0.01522899679361644</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59">
+        <v>14.04530482976033</v>
+      </c>
+      <c r="D59">
+        <v>0.01732375264552129</v>
+      </c>
+      <c r="E59">
+        <v>0.1935434560399775</v>
+      </c>
+      <c r="F59">
+        <v>24.32640549076017</v>
+      </c>
+      <c r="G59">
+        <v>0.9617869969330447</v>
+      </c>
+      <c r="H59">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I59">
+        <v>0.8297178064735136</v>
+      </c>
+      <c r="J59">
+        <v>0.0009817641687142262</v>
+      </c>
+      <c r="K59">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L59">
+        <v>0.8563907633913891</v>
+      </c>
+      <c r="M59">
+        <v>0.0003374352511826652</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60">
+        <v>13.63474381826463</v>
+      </c>
+      <c r="D60">
+        <v>0.01724864105781772</v>
+      </c>
+      <c r="E60">
+        <v>0.1986614816503784</v>
+      </c>
+      <c r="F60">
+        <v>23.61522714413747</v>
+      </c>
+      <c r="G60">
+        <v>0.9612612357341704</v>
+      </c>
+      <c r="H60">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I60">
+        <v>0.8442091077762766</v>
+      </c>
+      <c r="J60">
+        <v>0.01646642622738768</v>
+      </c>
+      <c r="K60">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L60">
+        <v>0.8748100758041264</v>
+      </c>
+      <c r="M60">
+        <v>0.02116337708185685</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61">
+        <v>14.57031810184137</v>
+      </c>
+      <c r="D61">
+        <v>0.02396667384109875</v>
+      </c>
+      <c r="E61">
+        <v>0.2106548752723834</v>
+      </c>
+      <c r="F61">
+        <v>25.23564064747731</v>
+      </c>
+      <c r="G61">
+        <v>0.9494547180826171</v>
+      </c>
+      <c r="H61">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I61">
+        <v>0.8520398164855043</v>
+      </c>
+      <c r="J61">
+        <v>0.02589495811975598</v>
+      </c>
+      <c r="K61">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L61">
+        <v>0.8706114959137968</v>
+      </c>
+      <c r="M61">
+        <v>0.01626238641160663</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62">
+        <v>14.57271107248556</v>
+      </c>
+      <c r="D62">
+        <v>0.0227214428366301</v>
+      </c>
+      <c r="E62">
+        <v>0.2155401264253553</v>
+      </c>
+      <c r="F62">
+        <v>25.23974544634648</v>
+      </c>
+      <c r="G62">
+        <v>0.9499557406407279</v>
+      </c>
+      <c r="H62">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I62">
+        <v>0.8423421832946056</v>
+      </c>
+      <c r="J62">
+        <v>0.01421856365585125</v>
+      </c>
+      <c r="K62">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L62">
+        <v>0.8593354494233968</v>
+      </c>
+      <c r="M62">
+        <v>0.003099888593226325</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63">
+        <v>13.69671475202967</v>
+      </c>
+      <c r="D63">
+        <v>0.01946534622255496</v>
+      </c>
+      <c r="E63">
+        <v>0.2055275252781552</v>
+      </c>
+      <c r="F63">
+        <v>23.72250755152273</v>
+      </c>
+      <c r="G63">
+        <v>0.9573261286493672</v>
+      </c>
+      <c r="H63">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I63">
+        <v>0.8399411018087091</v>
+      </c>
+      <c r="J63">
+        <v>0.01132755158956492</v>
+      </c>
+      <c r="K63">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L63">
+        <v>0.872445773897669</v>
+      </c>
+      <c r="M63">
+        <v>0.01840353401875556</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64">
+        <v>13.39616587238766</v>
+      </c>
+      <c r="D64">
+        <v>0.01972067094627941</v>
+      </c>
+      <c r="E64">
+        <v>0.1999885687332631</v>
+      </c>
+      <c r="F64">
+        <v>23.20196965580904</v>
+      </c>
+      <c r="G64">
+        <v>0.9586527242357832</v>
+      </c>
+      <c r="H64">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I64">
+        <v>0.8429406443900843</v>
+      </c>
+      <c r="J64">
+        <v>0.01493913822126869</v>
+      </c>
+      <c r="K64">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L64">
+        <v>0.8697026577855141</v>
+      </c>
+      <c r="M64">
+        <v>0.01520150218317017</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65">
+        <v>14.88730385540946</v>
+      </c>
+      <c r="D65">
+        <v>0.01898907590690929</v>
+      </c>
+      <c r="E65">
+        <v>0.2056681697307653</v>
+      </c>
+      <c r="F65">
+        <v>25.78473944543214</v>
+      </c>
+      <c r="G65">
+        <v>0.9562815497374598</v>
+      </c>
+      <c r="H65">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I65">
+        <v>0.8422287719812175</v>
+      </c>
+      <c r="J65">
+        <v>0.01408201124087308</v>
+      </c>
+      <c r="K65">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L65">
+        <v>0.8713534553070402</v>
+      </c>
+      <c r="M65">
+        <v>0.01712847355511099</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>57</v>
+      </c>
+      <c r="C66">
+        <v>14.39436702375389</v>
+      </c>
+      <c r="D66">
+        <v>0.02447590880355292</v>
+      </c>
+      <c r="E66">
+        <v>0.2046116611793118</v>
+      </c>
+      <c r="F66">
+        <v>24.93092338926899</v>
+      </c>
+      <c r="G66">
+        <v>0.9503717241243503</v>
+      </c>
+      <c r="H66">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I66">
+        <v>0.8399435796152546</v>
+      </c>
+      <c r="J66">
+        <v>0.01133053498211658</v>
+      </c>
+      <c r="K66">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L66">
+        <v>0.8666890707071662</v>
+      </c>
+      <c r="M66">
+        <v>0.01168375033831704</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>58</v>
+      </c>
+      <c r="C67">
+        <v>13.79941152897266</v>
+      </c>
+      <c r="D67">
+        <v>0.02008726036168429</v>
+      </c>
+      <c r="E67">
+        <v>0.2042522027301002</v>
+      </c>
+      <c r="F67">
+        <v>23.9004006907307</v>
+      </c>
+      <c r="G67">
+        <v>0.9567868923750725</v>
+      </c>
+      <c r="H67">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I67">
+        <v>0.8449143168525881</v>
+      </c>
+      <c r="J67">
+        <v>0.01731553025024014</v>
+      </c>
+      <c r="K67">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L67">
+        <v>0.8686754845254263</v>
+      </c>
+      <c r="M67">
+        <v>0.01400248568332555</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68">
+        <v>14.09323829269358</v>
+      </c>
+      <c r="D68">
+        <v>0.01932011451410275</v>
+      </c>
+      <c r="E68">
+        <v>0.1955122701938349</v>
+      </c>
+      <c r="F68">
+        <v>24.40941413490525</v>
+      </c>
+      <c r="G68">
+        <v>0.9592155250218797</v>
+      </c>
+      <c r="H68">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I68">
+        <v>0.8349020228458838</v>
+      </c>
+      <c r="J68">
+        <v>0.005260269754247368</v>
+      </c>
+      <c r="K68">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L68">
+        <v>0.8670925711389371</v>
+      </c>
+      <c r="M68">
+        <v>0.01215475527408263</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69">
+        <v>15.01665007030294</v>
+      </c>
+      <c r="D69">
+        <v>0.02286744267166354</v>
+      </c>
+      <c r="E69">
+        <v>0.2008323361797119</v>
+      </c>
+      <c r="F69">
+        <v>26.00881545658314</v>
+      </c>
+      <c r="G69">
+        <v>0.9525670422522529</v>
+      </c>
+      <c r="H69">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I69">
+        <v>0.8386944808551214</v>
+      </c>
+      <c r="J69">
+        <v>0.009826562872573722</v>
+      </c>
+      <c r="K69">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L69">
+        <v>0.8621056025981683</v>
+      </c>
+      <c r="M69">
+        <v>0.006333480717074976</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>60</v>
+      </c>
+      <c r="C70">
+        <v>14.24139231740931</v>
+      </c>
+      <c r="D70">
+        <v>0.01946198458448447</v>
+      </c>
+      <c r="E70">
+        <v>0.2176458001312462</v>
+      </c>
+      <c r="F70">
+        <v>24.6658471768544</v>
+      </c>
+      <c r="G70">
+        <v>0.9538018436528265</v>
+      </c>
+      <c r="H70">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I70">
+        <v>0.8371939201227347</v>
+      </c>
+      <c r="J70">
+        <v>0.00801981903276376</v>
+      </c>
+      <c r="K70">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L70">
+        <v>0.8656244945115483</v>
+      </c>
+      <c r="M70">
+        <v>0.01044107349548485</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71">
+        <v>14.76738229134054</v>
+      </c>
+      <c r="D71">
+        <v>0.01946406239818661</v>
+      </c>
+      <c r="E71">
+        <v>0.2091455153059497</v>
+      </c>
+      <c r="F71">
+        <v>25.57699393047384</v>
+      </c>
+      <c r="G71">
+        <v>0.9551217447067396</v>
+      </c>
+      <c r="H71">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I71">
+        <v>0.842985077637697</v>
+      </c>
+      <c r="J71">
+        <v>0.01499263788621017</v>
+      </c>
+      <c r="K71">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L71">
+        <v>0.8694052755876758</v>
+      </c>
+      <c r="M71">
+        <v>0.01485436876778339</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72">
+        <v>14.54182832060515</v>
+      </c>
+      <c r="D72">
+        <v>0.016850360553388</v>
+      </c>
+      <c r="E72">
+        <v>0.202619596292974</v>
+      </c>
+      <c r="F72">
+        <v>25.18636484454255</v>
+      </c>
+      <c r="G72">
+        <v>0.9596156952129834</v>
+      </c>
+      <c r="H72">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I72">
+        <v>0.8351377161837641</v>
+      </c>
+      <c r="J72">
+        <v>0.005544055326606176</v>
+      </c>
+      <c r="K72">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L72">
+        <v>0.8686627038174052</v>
+      </c>
+      <c r="M72">
+        <v>0.01398756679827229</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73">
+        <v>14.27119011972252</v>
+      </c>
+      <c r="D73">
+        <v>0.01812250089456627</v>
+      </c>
+      <c r="E73">
+        <v>0.1996080634261606</v>
+      </c>
+      <c r="F73">
+        <v>24.71761377026053</v>
+      </c>
+      <c r="G73">
+        <v>0.9593698706019138</v>
+      </c>
+      <c r="H73">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I73">
+        <v>0.8365588162552777</v>
+      </c>
+      <c r="J73">
+        <v>0.007255124891832612</v>
+      </c>
+      <c r="K73">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L73">
+        <v>0.8635918515878865</v>
+      </c>
+      <c r="M73">
+        <v>0.008068375043858007</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74">
+        <v>13.99502835485324</v>
+      </c>
+      <c r="D74">
+        <v>0.01796004899966564</v>
+      </c>
+      <c r="E74">
+        <v>0.2005388753804234</v>
+      </c>
+      <c r="F74">
+        <v>24.23926396480597</v>
+      </c>
+      <c r="G74">
+        <v>0.9596826829040381</v>
+      </c>
+      <c r="H74">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I74">
+        <v>0.8397540173044437</v>
+      </c>
+      <c r="J74">
+        <v>0.01110229327891473</v>
+      </c>
+      <c r="K74">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L74">
+        <v>0.8659893584487536</v>
+      </c>
+      <c r="M74">
+        <v>0.01086697815821911</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>62</v>
+      </c>
+      <c r="C75">
+        <v>13.3398519967597</v>
+      </c>
+      <c r="D75">
+        <v>0.0215575814299201</v>
+      </c>
+      <c r="E75">
+        <v>0.2123058184372958</v>
+      </c>
+      <c r="F75">
+        <v>23.10431594738312</v>
+      </c>
+      <c r="G75">
+        <v>0.9537441741764061</v>
+      </c>
+      <c r="H75">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I75">
+        <v>0.8400077852998619</v>
+      </c>
+      <c r="J75">
+        <v>0.01140784156667615</v>
+      </c>
+      <c r="K75">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L75">
+        <v>0.8643456494312902</v>
+      </c>
+      <c r="M75">
+        <v>0.008948281177425989</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>62</v>
+      </c>
+      <c r="C76">
+        <v>14.12600395549064</v>
+      </c>
+      <c r="D76">
+        <v>0.02192426947894117</v>
+      </c>
+      <c r="E76">
+        <v>0.2019342176091955</v>
+      </c>
+      <c r="F76">
+        <v>24.46611340507064</v>
+      </c>
+      <c r="G76">
+        <v>0.9546964668953991</v>
+      </c>
+      <c r="H76">
+        <v>0.8305331942045113</v>
+      </c>
+      <c r="I76">
+        <v>0.8449876401094213</v>
+      </c>
+      <c r="J76">
+        <v>0.0174038148092979</v>
+      </c>
+      <c r="K76">
+        <v>0.8566798373674943</v>
+      </c>
+      <c r="L76">
+        <v>0.8739531355613546</v>
+      </c>
+      <c r="M76">
+        <v>0.02016307311135004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>